<commit_message>
In the criteira.R file I made sure to pull out the criteria that show 0 as an artifact from excel in the applicable criteria data frame.
In the toxics analysis I switched back the data frame for the criteria evaluation to the data wo void so we could see the new methods included.

Not sure what changed with the data summary draft excel file. Learning that changes in xlsx files don't show up in the R studio diff.
</commit_message>
<xml_diff>
--- a/Draft Outputs/Data_Summary_DRAFT.xlsx
+++ b/Draft Outputs/Data_Summary_DRAFT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="570" windowWidth="18855" windowHeight="11700"/>
+    <workbookView xWindow="150" yWindow="570" windowWidth="18855" windowHeight="11700" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TotalDetects" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="524">
   <si>
     <t>Analyte</t>
   </si>
@@ -1628,8 +1628,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1867,24 +1868,24 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="77981184"/>
-        <c:axId val="77982720"/>
+        <c:axId val="76804864"/>
+        <c:axId val="76807168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="77981184"/>
+        <c:axId val="76804864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77982720"/>
+        <c:crossAx val="76807168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77982720"/>
+        <c:axId val="76807168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1892,20 +1893,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77981184"/>
+        <c:crossAx val="76804864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2234,7 +2234,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E270"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -9040,8 +9040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9098,8 +9098,8 @@
       <c r="A2" t="s">
         <v>290</v>
       </c>
-      <c r="B2" t="s">
-        <v>384</v>
+      <c r="B2" s="1">
+        <v>10411</v>
       </c>
       <c r="C2" t="s">
         <v>486</v>
@@ -9133,8 +9133,8 @@
       <c r="A3" t="s">
         <v>290</v>
       </c>
-      <c r="B3" t="s">
-        <v>358</v>
+      <c r="B3" s="1">
+        <v>10506</v>
       </c>
       <c r="C3" t="s">
         <v>460</v>
@@ -9168,8 +9168,8 @@
       <c r="A4" t="s">
         <v>290</v>
       </c>
-      <c r="B4" t="s">
-        <v>359</v>
+      <c r="B4" s="1">
+        <v>10508</v>
       </c>
       <c r="C4" t="s">
         <v>461</v>
@@ -9203,8 +9203,8 @@
       <c r="A5" t="s">
         <v>290</v>
       </c>
-      <c r="B5" t="s">
-        <v>325</v>
+      <c r="B5" s="1">
+        <v>10517</v>
       </c>
       <c r="C5" t="s">
         <v>427</v>
@@ -9238,8 +9238,8 @@
       <c r="A6" t="s">
         <v>290</v>
       </c>
-      <c r="B6" t="s">
-        <v>345</v>
+      <c r="B6" s="1">
+        <v>10684</v>
       </c>
       <c r="C6" t="s">
         <v>447</v>
@@ -9273,8 +9273,8 @@
       <c r="A7" t="s">
         <v>290</v>
       </c>
-      <c r="B7" t="s">
-        <v>338</v>
+      <c r="B7" s="1">
+        <v>10689</v>
       </c>
       <c r="C7" t="s">
         <v>440</v>
@@ -9308,8 +9308,8 @@
       <c r="A8" t="s">
         <v>290</v>
       </c>
-      <c r="B8" t="s">
-        <v>346</v>
+      <c r="B8" s="1">
+        <v>10696</v>
       </c>
       <c r="C8" t="s">
         <v>448</v>
@@ -9343,8 +9343,8 @@
       <c r="A9" t="s">
         <v>290</v>
       </c>
-      <c r="B9" t="s">
-        <v>339</v>
+      <c r="B9" s="1">
+        <v>10697</v>
       </c>
       <c r="C9" t="s">
         <v>441</v>
@@ -9378,8 +9378,8 @@
       <c r="A10" t="s">
         <v>290</v>
       </c>
-      <c r="B10" t="s">
-        <v>347</v>
+      <c r="B10" s="1">
+        <v>11387</v>
       </c>
       <c r="C10" t="s">
         <v>449</v>
@@ -9413,8 +9413,8 @@
       <c r="A11" t="s">
         <v>290</v>
       </c>
-      <c r="B11" t="s">
-        <v>362</v>
+      <c r="B11" s="1">
+        <v>11477</v>
       </c>
       <c r="C11" t="s">
         <v>464</v>
@@ -9448,8 +9448,8 @@
       <c r="A12" t="s">
         <v>290</v>
       </c>
-      <c r="B12" t="s">
-        <v>363</v>
+      <c r="B12" s="1">
+        <v>12561</v>
       </c>
       <c r="C12" t="s">
         <v>465</v>
@@ -9483,8 +9483,8 @@
       <c r="A13" t="s">
         <v>290</v>
       </c>
-      <c r="B13" t="s">
-        <v>385</v>
+      <c r="B13" s="1">
+        <v>25558</v>
       </c>
       <c r="C13" t="s">
         <v>487</v>
@@ -9518,8 +9518,8 @@
       <c r="A14" t="s">
         <v>290</v>
       </c>
-      <c r="B14" t="s">
-        <v>340</v>
+      <c r="B14" s="1">
+        <v>32475</v>
       </c>
       <c r="C14" t="s">
         <v>442</v>
@@ -9553,8 +9553,8 @@
       <c r="A15" t="s">
         <v>290</v>
       </c>
-      <c r="B15" t="s">
-        <v>326</v>
+      <c r="B15" s="1">
+        <v>32494</v>
       </c>
       <c r="C15" t="s">
         <v>428</v>
@@ -9588,8 +9588,8 @@
       <c r="A16" t="s">
         <v>290</v>
       </c>
-      <c r="B16" t="s">
-        <v>364</v>
+      <c r="B16" s="1">
+        <v>33093</v>
       </c>
       <c r="C16" t="s">
         <v>466</v>
@@ -9623,8 +9623,8 @@
       <c r="A17" t="s">
         <v>290</v>
       </c>
-      <c r="B17" t="s">
-        <v>365</v>
+      <c r="B17" s="1">
+        <v>33939</v>
       </c>
       <c r="C17" t="s">
         <v>467</v>
@@ -9658,8 +9658,8 @@
       <c r="A18" t="s">
         <v>290</v>
       </c>
-      <c r="B18" t="s">
-        <v>377</v>
+      <c r="B18" s="1">
+        <v>36030</v>
       </c>
       <c r="C18" t="s">
         <v>479</v>
@@ -9693,8 +9693,8 @@
       <c r="A19" t="s">
         <v>290</v>
       </c>
-      <c r="B19" t="s">
-        <v>317</v>
+      <c r="B19" s="1">
+        <v>36776</v>
       </c>
       <c r="C19" t="s">
         <v>419</v>
@@ -9728,8 +9728,8 @@
       <c r="A20" t="s">
         <v>290</v>
       </c>
-      <c r="B20" t="s">
-        <v>378</v>
+      <c r="B20" s="1">
+        <v>37106</v>
       </c>
       <c r="C20" t="s">
         <v>480</v>
@@ -9763,8 +9763,8 @@
       <c r="A21" t="s">
         <v>286</v>
       </c>
-      <c r="B21" t="s">
-        <v>366</v>
+      <c r="B21" s="1">
+        <v>10674</v>
       </c>
       <c r="C21" t="s">
         <v>468</v>
@@ -9798,8 +9798,8 @@
       <c r="A22" t="s">
         <v>286</v>
       </c>
-      <c r="B22" t="s">
-        <v>394</v>
+      <c r="B22" s="1">
+        <v>11025</v>
       </c>
       <c r="C22" t="s">
         <v>496</v>
@@ -9833,8 +9833,8 @@
       <c r="A23" t="s">
         <v>286</v>
       </c>
-      <c r="B23" t="s">
-        <v>300</v>
+      <c r="B23" s="1">
+        <v>11972</v>
       </c>
       <c r="C23" t="s">
         <v>402</v>
@@ -9868,8 +9868,8 @@
       <c r="A24" t="s">
         <v>286</v>
       </c>
-      <c r="B24" t="s">
-        <v>386</v>
+      <c r="B24" s="1">
+        <v>12012</v>
       </c>
       <c r="C24" t="s">
         <v>488</v>
@@ -9903,8 +9903,8 @@
       <c r="A25" t="s">
         <v>286</v>
       </c>
-      <c r="B25" t="s">
-        <v>341</v>
+      <c r="B25" s="1">
+        <v>12550</v>
       </c>
       <c r="C25" t="s">
         <v>443</v>
@@ -9938,8 +9938,8 @@
       <c r="A26" t="s">
         <v>286</v>
       </c>
-      <c r="B26" t="s">
-        <v>371</v>
+      <c r="B26" s="1">
+        <v>13138</v>
       </c>
       <c r="C26" t="s">
         <v>473</v>
@@ -9973,8 +9973,8 @@
       <c r="A27" t="s">
         <v>286</v>
       </c>
-      <c r="B27" t="s">
-        <v>372</v>
+      <c r="B27" s="1">
+        <v>13139</v>
       </c>
       <c r="C27" t="s">
         <v>474</v>
@@ -10008,8 +10008,8 @@
       <c r="A28" t="s">
         <v>286</v>
       </c>
-      <c r="B28" t="s">
-        <v>397</v>
+      <c r="B28" s="1">
+        <v>13140</v>
       </c>
       <c r="C28" t="s">
         <v>499</v>
@@ -10043,8 +10043,8 @@
       <c r="A29" t="s">
         <v>286</v>
       </c>
-      <c r="B29" t="s">
-        <v>318</v>
+      <c r="B29" s="1">
+        <v>13141</v>
       </c>
       <c r="C29" t="s">
         <v>420</v>
@@ -10078,8 +10078,8 @@
       <c r="A30" t="s">
         <v>286</v>
       </c>
-      <c r="B30" t="s">
-        <v>319</v>
+      <c r="B30" s="1">
+        <v>13148</v>
       </c>
       <c r="C30" t="s">
         <v>421</v>
@@ -10113,8 +10113,8 @@
       <c r="A31" t="s">
         <v>286</v>
       </c>
-      <c r="B31" t="s">
-        <v>310</v>
+      <c r="B31" s="1">
+        <v>13253</v>
       </c>
       <c r="C31" t="s">
         <v>412</v>
@@ -10148,8 +10148,8 @@
       <c r="A32" t="s">
         <v>286</v>
       </c>
-      <c r="B32" t="s">
-        <v>302</v>
+      <c r="B32" s="1">
+        <v>25204</v>
       </c>
       <c r="C32" t="s">
         <v>404</v>
@@ -10183,8 +10183,8 @@
       <c r="A33" t="s">
         <v>286</v>
       </c>
-      <c r="B33" t="s">
-        <v>387</v>
+      <c r="B33" s="1">
+        <v>26419</v>
       </c>
       <c r="C33" t="s">
         <v>489</v>
@@ -10218,8 +10218,8 @@
       <c r="A34" t="s">
         <v>286</v>
       </c>
-      <c r="B34" t="s">
-        <v>311</v>
+      <c r="B34" s="1">
+        <v>28333</v>
       </c>
       <c r="C34" t="s">
         <v>413</v>
@@ -10253,8 +10253,8 @@
       <c r="A35" t="s">
         <v>286</v>
       </c>
-      <c r="B35" t="s">
-        <v>327</v>
+      <c r="B35" s="1">
+        <v>28574</v>
       </c>
       <c r="C35" t="s">
         <v>429</v>
@@ -10288,8 +10288,8 @@
       <c r="A36" t="s">
         <v>286</v>
       </c>
-      <c r="B36" t="s">
-        <v>395</v>
+      <c r="B36" s="1">
+        <v>32982</v>
       </c>
       <c r="C36" t="s">
         <v>497</v>
@@ -10323,8 +10323,8 @@
       <c r="A37" t="s">
         <v>286</v>
       </c>
-      <c r="B37" t="s">
-        <v>307</v>
+      <c r="B37" s="1">
+        <v>34102</v>
       </c>
       <c r="C37" t="s">
         <v>409</v>
@@ -10358,8 +10358,8 @@
       <c r="A38" t="s">
         <v>286</v>
       </c>
-      <c r="B38" t="s">
-        <v>304</v>
+      <c r="B38" s="1">
+        <v>37091</v>
       </c>
       <c r="C38" t="s">
         <v>406</v>
@@ -10393,8 +10393,8 @@
       <c r="A39" t="s">
         <v>291</v>
       </c>
-      <c r="B39" t="s">
-        <v>367</v>
+      <c r="B39" s="1">
+        <v>11016</v>
       </c>
       <c r="C39" t="s">
         <v>469</v>
@@ -10428,8 +10428,8 @@
       <c r="A40" t="s">
         <v>291</v>
       </c>
-      <c r="B40" t="s">
-        <v>388</v>
+      <c r="B40" s="1">
+        <v>11020</v>
       </c>
       <c r="C40" t="s">
         <v>490</v>
@@ -10463,8 +10463,8 @@
       <c r="A41" t="s">
         <v>291</v>
       </c>
-      <c r="B41" t="s">
-        <v>379</v>
+      <c r="B41" s="1">
+        <v>11386</v>
       </c>
       <c r="C41" t="s">
         <v>481</v>
@@ -10498,8 +10498,8 @@
       <c r="A42" t="s">
         <v>291</v>
       </c>
-      <c r="B42" t="s">
-        <v>328</v>
+      <c r="B42" s="1">
+        <v>11478</v>
       </c>
       <c r="C42" t="s">
         <v>430</v>
@@ -10533,8 +10533,8 @@
       <c r="A43" t="s">
         <v>291</v>
       </c>
-      <c r="B43" t="s">
-        <v>329</v>
+      <c r="B43" s="1">
+        <v>24135</v>
       </c>
       <c r="C43" t="s">
         <v>431</v>
@@ -10568,8 +10568,8 @@
       <c r="A44" t="s">
         <v>291</v>
       </c>
-      <c r="B44" t="s">
-        <v>348</v>
+      <c r="B44" s="1">
+        <v>31987</v>
       </c>
       <c r="C44" t="s">
         <v>450</v>
@@ -10603,8 +10603,8 @@
       <c r="A45" t="s">
         <v>291</v>
       </c>
-      <c r="B45" t="s">
-        <v>368</v>
+      <c r="B45" s="1">
+        <v>31990</v>
       </c>
       <c r="C45" t="s">
         <v>470</v>
@@ -10638,8 +10638,8 @@
       <c r="A46" t="s">
         <v>291</v>
       </c>
-      <c r="B46" t="s">
-        <v>373</v>
+      <c r="B46" s="1">
+        <v>36787</v>
       </c>
       <c r="C46" t="s">
         <v>475</v>
@@ -10673,8 +10673,8 @@
       <c r="A47" t="s">
         <v>291</v>
       </c>
-      <c r="B47" t="s">
-        <v>380</v>
+      <c r="B47" s="1">
+        <v>37118</v>
       </c>
       <c r="C47" t="s">
         <v>482</v>
@@ -10708,8 +10708,8 @@
       <c r="A48" t="s">
         <v>291</v>
       </c>
-      <c r="B48" t="s">
-        <v>360</v>
+      <c r="B48" s="1">
+        <v>37135</v>
       </c>
       <c r="C48" t="s">
         <v>462</v>
@@ -10743,8 +10743,8 @@
       <c r="A49" t="s">
         <v>293</v>
       </c>
-      <c r="B49" t="s">
-        <v>349</v>
+      <c r="B49" s="1">
+        <v>10719</v>
       </c>
       <c r="C49" t="s">
         <v>451</v>
@@ -10778,8 +10778,8 @@
       <c r="A50" t="s">
         <v>293</v>
       </c>
-      <c r="B50" t="s">
-        <v>389</v>
+      <c r="B50" s="1">
+        <v>10720</v>
       </c>
       <c r="C50" t="s">
         <v>491</v>
@@ -10813,8 +10813,8 @@
       <c r="A51" t="s">
         <v>293</v>
       </c>
-      <c r="B51" t="s">
-        <v>390</v>
+      <c r="B51" s="1">
+        <v>11521</v>
       </c>
       <c r="C51" t="s">
         <v>492</v>
@@ -10848,8 +10848,8 @@
       <c r="A52" t="s">
         <v>294</v>
       </c>
-      <c r="B52" t="s">
-        <v>350</v>
+      <c r="B52" s="1">
+        <v>10759</v>
       </c>
       <c r="C52" t="s">
         <v>452</v>
@@ -10883,8 +10883,8 @@
       <c r="A53" t="s">
         <v>294</v>
       </c>
-      <c r="B53" t="s">
-        <v>351</v>
+      <c r="B53" s="1">
+        <v>10763</v>
       </c>
       <c r="C53" t="s">
         <v>453</v>
@@ -10918,8 +10918,8 @@
       <c r="A54" t="s">
         <v>294</v>
       </c>
-      <c r="B54" t="s">
-        <v>391</v>
+      <c r="B54" s="1">
+        <v>10765</v>
       </c>
       <c r="C54" t="s">
         <v>493</v>
@@ -10953,8 +10953,8 @@
       <c r="A55" t="s">
         <v>294</v>
       </c>
-      <c r="B55" t="s">
-        <v>392</v>
+      <c r="B55" s="1">
+        <v>10768</v>
       </c>
       <c r="C55" t="s">
         <v>494</v>
@@ -10988,8 +10988,8 @@
       <c r="A56" t="s">
         <v>294</v>
       </c>
-      <c r="B56" t="s">
-        <v>381</v>
+      <c r="B56" s="1">
+        <v>10770</v>
       </c>
       <c r="C56" t="s">
         <v>483</v>
@@ -11023,8 +11023,8 @@
       <c r="A57" t="s">
         <v>287</v>
       </c>
-      <c r="B57" t="s">
-        <v>305</v>
+      <c r="B57" s="1">
+        <v>10407</v>
       </c>
       <c r="C57" t="s">
         <v>407</v>
@@ -11058,8 +11058,8 @@
       <c r="A58" t="s">
         <v>287</v>
       </c>
-      <c r="B58" t="s">
-        <v>342</v>
+      <c r="B58" s="1">
+        <v>11480</v>
       </c>
       <c r="C58" t="s">
         <v>444</v>
@@ -11093,8 +11093,8 @@
       <c r="A59" t="s">
         <v>285</v>
       </c>
-      <c r="B59" t="s">
-        <v>299</v>
+      <c r="B59" s="1">
+        <v>10729</v>
       </c>
       <c r="C59" t="s">
         <v>401</v>
@@ -11128,8 +11128,8 @@
       <c r="A60" t="s">
         <v>292</v>
       </c>
-      <c r="B60" t="s">
-        <v>335</v>
+      <c r="B60" s="1">
+        <v>10724</v>
       </c>
       <c r="C60" t="s">
         <v>437</v>
@@ -11163,8 +11163,8 @@
       <c r="A61" t="s">
         <v>292</v>
       </c>
-      <c r="B61" t="s">
-        <v>330</v>
+      <c r="B61" s="1">
+        <v>11494</v>
       </c>
       <c r="C61" t="s">
         <v>432</v>
@@ -11198,8 +11198,8 @@
       <c r="A62" t="s">
         <v>292</v>
       </c>
-      <c r="B62" t="s">
-        <v>331</v>
+      <c r="B62" s="1">
+        <v>11857</v>
       </c>
       <c r="C62" t="s">
         <v>433</v>
@@ -11233,8 +11233,8 @@
       <c r="A63" t="s">
         <v>289</v>
       </c>
-      <c r="B63" t="s">
-        <v>336</v>
+      <c r="B63" s="1">
+        <v>10418</v>
       </c>
       <c r="C63" t="s">
         <v>438</v>
@@ -11268,8 +11268,8 @@
       <c r="A64" t="s">
         <v>289</v>
       </c>
-      <c r="B64" t="s">
-        <v>374</v>
+      <c r="B64" s="1">
+        <v>10423</v>
       </c>
       <c r="C64" t="s">
         <v>476</v>
@@ -11303,8 +11303,8 @@
       <c r="A65" t="s">
         <v>289</v>
       </c>
-      <c r="B65" t="s">
-        <v>352</v>
+      <c r="B65" s="1">
+        <v>10428</v>
       </c>
       <c r="C65" t="s">
         <v>454</v>
@@ -11338,8 +11338,8 @@
       <c r="A66" t="s">
         <v>289</v>
       </c>
-      <c r="B66" t="s">
-        <v>312</v>
+      <c r="B66" s="1">
+        <v>10434</v>
       </c>
       <c r="C66" t="s">
         <v>414</v>
@@ -11373,8 +11373,8 @@
       <c r="A67" t="s">
         <v>289</v>
       </c>
-      <c r="B67" t="s">
-        <v>353</v>
+      <c r="B67" s="1">
+        <v>10602</v>
       </c>
       <c r="C67" t="s">
         <v>455</v>
@@ -11408,8 +11408,8 @@
       <c r="A68" t="s">
         <v>289</v>
       </c>
-      <c r="B68" t="s">
-        <v>320</v>
+      <c r="B68" s="1">
+        <v>11051</v>
       </c>
       <c r="C68" t="s">
         <v>422</v>
@@ -11443,8 +11443,8 @@
       <c r="A69" t="s">
         <v>289</v>
       </c>
-      <c r="B69" t="s">
-        <v>375</v>
+      <c r="B69" s="1">
+        <v>11375</v>
       </c>
       <c r="C69" t="s">
         <v>477</v>
@@ -11478,8 +11478,8 @@
       <c r="A70" t="s">
         <v>289</v>
       </c>
-      <c r="B70" t="s">
-        <v>354</v>
+      <c r="B70" s="1">
+        <v>11482</v>
       </c>
       <c r="C70" t="s">
         <v>456</v>
@@ -11513,8 +11513,8 @@
       <c r="A71" t="s">
         <v>289</v>
       </c>
-      <c r="B71" t="s">
-        <v>361</v>
+      <c r="B71" s="1">
+        <v>34860</v>
       </c>
       <c r="C71" t="s">
         <v>463</v>
@@ -11548,8 +11548,8 @@
       <c r="A72" t="s">
         <v>288</v>
       </c>
-      <c r="B72" t="s">
-        <v>323</v>
+      <c r="B72" s="1">
+        <v>10404</v>
       </c>
       <c r="C72" t="s">
         <v>425</v>
@@ -11583,8 +11583,8 @@
       <c r="A73" t="s">
         <v>288</v>
       </c>
-      <c r="B73" t="s">
-        <v>396</v>
+      <c r="B73" s="1">
+        <v>10406</v>
       </c>
       <c r="C73" t="s">
         <v>498</v>
@@ -11618,8 +11618,8 @@
       <c r="A74" t="s">
         <v>288</v>
       </c>
-      <c r="B74" t="s">
-        <v>308</v>
+      <c r="B74" s="1">
+        <v>10708</v>
       </c>
       <c r="C74" t="s">
         <v>410</v>
@@ -11653,8 +11653,8 @@
       <c r="A75" t="s">
         <v>288</v>
       </c>
-      <c r="B75" t="s">
-        <v>321</v>
+      <c r="B75" s="1">
+        <v>11489</v>
       </c>
       <c r="C75" t="s">
         <v>423</v>
@@ -11688,8 +11688,8 @@
       <c r="A76" t="s">
         <v>288</v>
       </c>
-      <c r="B76" t="s">
-        <v>332</v>
+      <c r="B76" s="1">
+        <v>12005</v>
       </c>
       <c r="C76" t="s">
         <v>434</v>
@@ -11723,8 +11723,8 @@
       <c r="A77" t="s">
         <v>288</v>
       </c>
-      <c r="B77" t="s">
-        <v>306</v>
+      <c r="B77" s="1">
+        <v>12015</v>
       </c>
       <c r="C77" t="s">
         <v>408</v>
@@ -11758,8 +11758,8 @@
       <c r="A78" t="s">
         <v>288</v>
       </c>
-      <c r="B78" t="s">
-        <v>314</v>
+      <c r="B78" s="1">
+        <v>36445</v>
       </c>
       <c r="C78" t="s">
         <v>416</v>
@@ -11793,8 +11793,8 @@
       <c r="A79" t="s">
         <v>295</v>
       </c>
-      <c r="B79" t="s">
-        <v>355</v>
+      <c r="B79" s="1">
+        <v>10442</v>
       </c>
       <c r="C79" t="s">
         <v>457</v>
@@ -11828,8 +11828,8 @@
       <c r="A80" t="s">
         <v>295</v>
       </c>
-      <c r="B80" t="s">
-        <v>382</v>
+      <c r="B80" s="1">
+        <v>10451</v>
       </c>
       <c r="C80" t="s">
         <v>484</v>
@@ -11863,8 +11863,8 @@
       <c r="A81" t="s">
         <v>295</v>
       </c>
-      <c r="B81" t="s">
-        <v>376</v>
+      <c r="B81" s="1">
+        <v>10997</v>
       </c>
       <c r="C81" t="s">
         <v>478</v>
@@ -11898,8 +11898,8 @@
       <c r="A82" t="s">
         <v>295</v>
       </c>
-      <c r="B82" t="s">
-        <v>383</v>
+      <c r="B82" s="1">
+        <v>11484</v>
       </c>
       <c r="C82" t="s">
         <v>485</v>
@@ -11933,8 +11933,8 @@
       <c r="A83" t="s">
         <v>296</v>
       </c>
-      <c r="B83" t="s">
-        <v>393</v>
+      <c r="B83" s="1">
+        <v>23497</v>
       </c>
       <c r="C83" t="s">
         <v>495</v>
@@ -11968,8 +11968,8 @@
       <c r="A84" t="s">
         <v>284</v>
       </c>
-      <c r="B84" t="s">
-        <v>303</v>
+      <c r="B84" s="1">
+        <v>10339</v>
       </c>
       <c r="C84" t="s">
         <v>405</v>
@@ -12003,8 +12003,8 @@
       <c r="A85" t="s">
         <v>284</v>
       </c>
-      <c r="B85" t="s">
-        <v>315</v>
+      <c r="B85" s="1">
+        <v>10344</v>
       </c>
       <c r="C85" t="s">
         <v>417</v>
@@ -12038,8 +12038,8 @@
       <c r="A86" t="s">
         <v>284</v>
       </c>
-      <c r="B86" t="s">
-        <v>337</v>
+      <c r="B86" s="1">
+        <v>10350</v>
       </c>
       <c r="C86" t="s">
         <v>439</v>
@@ -12073,8 +12073,8 @@
       <c r="A87" t="s">
         <v>284</v>
       </c>
-      <c r="B87" t="s">
-        <v>322</v>
+      <c r="B87" s="1">
+        <v>10352</v>
       </c>
       <c r="C87" t="s">
         <v>424</v>
@@ -12108,8 +12108,8 @@
       <c r="A88" t="s">
         <v>284</v>
       </c>
-      <c r="B88" t="s">
-        <v>356</v>
+      <c r="B88" s="1">
+        <v>10355</v>
       </c>
       <c r="C88" t="s">
         <v>458</v>
@@ -12143,8 +12143,8 @@
       <c r="A89" t="s">
         <v>284</v>
       </c>
-      <c r="B89" t="s">
-        <v>398</v>
+      <c r="B89" s="1">
+        <v>10360</v>
       </c>
       <c r="C89" t="s">
         <v>500</v>
@@ -12178,8 +12178,8 @@
       <c r="A90" t="s">
         <v>284</v>
       </c>
-      <c r="B90" t="s">
-        <v>301</v>
+      <c r="B90" s="1">
+        <v>10363</v>
       </c>
       <c r="C90" t="s">
         <v>403</v>
@@ -12213,8 +12213,8 @@
       <c r="A91" t="s">
         <v>284</v>
       </c>
-      <c r="B91" t="s">
-        <v>357</v>
+      <c r="B91" s="1">
+        <v>10366</v>
       </c>
       <c r="C91" t="s">
         <v>459</v>
@@ -12248,8 +12248,8 @@
       <c r="A92" t="s">
         <v>284</v>
       </c>
-      <c r="B92" t="s">
-        <v>333</v>
+      <c r="B92" s="1">
+        <v>10373</v>
       </c>
       <c r="C92" t="s">
         <v>435</v>
@@ -12283,8 +12283,8 @@
       <c r="A93" t="s">
         <v>284</v>
       </c>
-      <c r="B93" t="s">
-        <v>369</v>
+      <c r="B93" s="1">
+        <v>10376</v>
       </c>
       <c r="C93" t="s">
         <v>471</v>
@@ -12318,8 +12318,8 @@
       <c r="A94" t="s">
         <v>284</v>
       </c>
-      <c r="B94" t="s">
-        <v>370</v>
+      <c r="B94" s="1">
+        <v>10386</v>
       </c>
       <c r="C94" t="s">
         <v>472</v>
@@ -12353,8 +12353,8 @@
       <c r="A95" t="s">
         <v>284</v>
       </c>
-      <c r="B95" t="s">
-        <v>297</v>
+      <c r="B95" s="1">
+        <v>10456</v>
       </c>
       <c r="C95" t="s">
         <v>399</v>
@@ -12388,8 +12388,8 @@
       <c r="A96" t="s">
         <v>284</v>
       </c>
-      <c r="B96" t="s">
-        <v>324</v>
+      <c r="B96" s="1">
+        <v>10555</v>
       </c>
       <c r="C96" t="s">
         <v>426</v>
@@ -12423,8 +12423,8 @@
       <c r="A97" t="s">
         <v>284</v>
       </c>
-      <c r="B97" t="s">
-        <v>309</v>
+      <c r="B97" s="1">
+        <v>10611</v>
       </c>
       <c r="C97" t="s">
         <v>411</v>
@@ -12458,8 +12458,8 @@
       <c r="A98" t="s">
         <v>284</v>
       </c>
-      <c r="B98" t="s">
-        <v>343</v>
+      <c r="B98" s="1">
+        <v>10637</v>
       </c>
       <c r="C98" t="s">
         <v>445</v>
@@ -12493,8 +12493,8 @@
       <c r="A99" t="s">
         <v>284</v>
       </c>
-      <c r="B99" t="s">
-        <v>298</v>
+      <c r="B99" s="1">
+        <v>10640</v>
       </c>
       <c r="C99" t="s">
         <v>400</v>
@@ -12528,8 +12528,8 @@
       <c r="A100" t="s">
         <v>284</v>
       </c>
-      <c r="B100" t="s">
-        <v>344</v>
+      <c r="B100" s="1">
+        <v>10792</v>
       </c>
       <c r="C100" t="s">
         <v>446</v>
@@ -12563,8 +12563,8 @@
       <c r="A101" t="s">
         <v>284</v>
       </c>
-      <c r="B101" t="s">
-        <v>316</v>
+      <c r="B101" s="1">
+        <v>11140</v>
       </c>
       <c r="C101" t="s">
         <v>418</v>
@@ -12598,8 +12598,8 @@
       <c r="A102" t="s">
         <v>284</v>
       </c>
-      <c r="B102" t="s">
-        <v>313</v>
+      <c r="B102" s="1">
+        <v>11180</v>
       </c>
       <c r="C102" t="s">
         <v>415</v>
@@ -12633,8 +12633,8 @@
       <c r="A103" t="s">
         <v>284</v>
       </c>
-      <c r="B103" t="s">
-        <v>334</v>
+      <c r="B103" s="1">
+        <v>11275</v>
       </c>
       <c r="C103" t="s">
         <v>436</v>

</xml_diff>